<commit_message>
update algorithms, strikes 1/19
</commit_message>
<xml_diff>
--- a/inputs/cwl-responses.xlsx
+++ b/inputs/cwl-responses.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>Timestamp</t>
   </si>
@@ -37,22 +37,43 @@
     <t>BB Crazy</t>
   </si>
   <si>
+    <t>8 stars only</t>
+  </si>
+  <si>
+    <t>Sned</t>
+  </si>
+  <si>
+    <t>BumblinMumbler</t>
+  </si>
+  <si>
+    <t>¯\_(ツ)_/¯</t>
+  </si>
+  <si>
+    <t>Genghis Khan</t>
+  </si>
+  <si>
+    <t>Taycid</t>
+  </si>
+  <si>
+    <t>Dr Stone</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
     <t>All 7 wars</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>BumblinMumbler</t>
-  </si>
-  <si>
-    <t>Icebreaker261</t>
-  </si>
-  <si>
-    <t>pg</t>
-  </si>
-  <si>
-    <t>I’m huge</t>
+    <t>So YUGE</t>
+  </si>
+  <si>
+    <t>Satan</t>
+  </si>
+  <si>
+    <t>Erdnussflip</t>
+  </si>
+  <si>
+    <t>Yo</t>
   </si>
   <si>
     <t>Protips</t>
@@ -61,111 +82,126 @@
     <t>Redking</t>
   </si>
   <si>
-    <t>Satan</t>
+    <t>Rious</t>
   </si>
   <si>
     <t>Smitty</t>
   </si>
   <si>
-    <t>Sned</t>
-  </si>
-  <si>
     <t>ERDNUSSFLIP</t>
   </si>
   <si>
-    <t>Yo</t>
+    <t>ImagineWaggons</t>
+  </si>
+  <si>
+    <t>K.L.A.U.S</t>
+  </si>
+  <si>
+    <t>Marlec</t>
+  </si>
+  <si>
+    <t>osiris8282</t>
+  </si>
+  <si>
+    <t>updating th level</t>
+  </si>
+  <si>
+    <t>RoyalOne</t>
+  </si>
+  <si>
+    <t>Welli</t>
+  </si>
+  <si>
+    <t>Anas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascended </t>
+  </si>
+  <si>
+    <t>GLHF</t>
+  </si>
+  <si>
+    <t>Koshal</t>
+  </si>
+  <si>
+    <t>Nope</t>
+  </si>
+  <si>
+    <t>Vojt</t>
+  </si>
+  <si>
+    <t>⚡ TANJIRO ⚡</t>
+  </si>
+  <si>
+    <t>DNG</t>
+  </si>
+  <si>
+    <t>Motz</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>Updating my TH level, hadn’t noticed my prior registration  was a while ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TruthfulLies </t>
+  </si>
+  <si>
+    <t>Vicream</t>
+  </si>
+  <si>
+    <t>CrazyWaveIT</t>
+  </si>
+  <si>
+    <t>I’m not that good at attacking bases but I’ll do my best</t>
+  </si>
+  <si>
+    <t>NagaStoleMyBike</t>
+  </si>
+  <si>
+    <t>&lt;3</t>
+  </si>
+  <si>
+    <t>Carsonn</t>
+  </si>
+  <si>
+    <t>None (participation medals only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All hero’s are upgrading need to be taken out </t>
+  </si>
+  <si>
+    <t>Jy</t>
+  </si>
+  <si>
+    <t>gdfan75</t>
+  </si>
+  <si>
+    <t>Matanza</t>
+  </si>
+  <si>
+    <t>Do not include me as filler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChrisThe7th </t>
+  </si>
+  <si>
+    <t>shadow</t>
+  </si>
+  <si>
+    <t>busy with uni :/</t>
   </si>
   <si>
     <t>Hype</t>
   </si>
   <si>
-    <t>ImagineWaggons</t>
-  </si>
-  <si>
-    <t>K.L.A.U.S</t>
-  </si>
-  <si>
-    <t>Marlec</t>
-  </si>
-  <si>
-    <t>Rious</t>
-  </si>
-  <si>
-    <t>Anas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascended </t>
-  </si>
-  <si>
-    <t>GLHF</t>
-  </si>
-  <si>
-    <t>Carsonn</t>
-  </si>
-  <si>
-    <t>RoyalOne</t>
-  </si>
-  <si>
-    <t>Vojt</t>
-  </si>
-  <si>
-    <t>Welli</t>
-  </si>
-  <si>
-    <t>DNG</t>
-  </si>
-  <si>
-    <t>Mythos</t>
-  </si>
-  <si>
-    <t>Rod</t>
-  </si>
-  <si>
-    <t>Updating my TH level, hadn’t noticed my prior registration  was a while ago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TruthfulLies </t>
-  </si>
-  <si>
-    <t>Vicream</t>
-  </si>
-  <si>
-    <t>CrazyWaveIT</t>
-  </si>
-  <si>
-    <t>I’m not that good at attacking bases but I’ll do my best</t>
-  </si>
-  <si>
-    <t>NagaStoleMyBike</t>
-  </si>
-  <si>
-    <t>&lt;3</t>
-  </si>
-  <si>
-    <t>osiris8282</t>
-  </si>
-  <si>
-    <t>Taycid</t>
-  </si>
-  <si>
-    <t>Apollo</t>
-  </si>
-  <si>
-    <t>Fresh TH12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ripexfruit </t>
-  </si>
-  <si>
-    <t>slothnz</t>
+    <t>Standby / bench</t>
   </si>
   <si>
     <t>Truthful Lies</t>
   </si>
   <si>
-    <t>As needed (alt account / filler)</t>
-  </si>
-  <si>
     <t>Will be upgrading th and heroes during hammer jam</t>
   </si>
   <si>
@@ -175,34 +211,10 @@
     <t>Please ping on Discord or in-game clan chat if put in for CWL. Thanks :)</t>
   </si>
   <si>
-    <t>⚡ TANJIRO ⚡</t>
-  </si>
-  <si>
-    <t>Dr. Stone</t>
-  </si>
-  <si>
     <t>Skyeshade</t>
   </si>
   <si>
     <t>BumblinMumbler2</t>
-  </si>
-  <si>
-    <t>Jy</t>
-  </si>
-  <si>
-    <t>None (participation medals only)</t>
-  </si>
-  <si>
-    <t>gdfan75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChrisThe7th </t>
-  </si>
-  <si>
-    <t>shadow</t>
-  </si>
-  <si>
-    <t>busy with uni :/</t>
   </si>
 </sst>
 </file>
@@ -296,13 +308,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,10 +652,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
-        <v>45930.81104166667</v>
+        <v>45992.512453703705</v>
       </c>
       <c r="B2" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -651,46 +663,46 @@
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="E2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4">
-        <v>45680.474224537036</v>
+        <v>45992.53902777778</v>
       </c>
       <c r="B3" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="22.5">
       <c r="A4" s="4">
-        <v>45953.02630787037</v>
+        <v>45971.73886574074</v>
       </c>
       <c r="B4" s="5">
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4">
-        <v>45952.146898148145</v>
+        <v>45992.512291666666</v>
       </c>
       <c r="B5" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -698,19 +710,17 @@
       <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4">
-        <v>45833.89664351852</v>
+        <v>45992.74783564815</v>
       </c>
       <c r="B6" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>6</v>
@@ -719,13 +729,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4">
-        <v>45961.168032407404</v>
+        <v>46019.11481481481</v>
       </c>
       <c r="B7" s="5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>6</v>
@@ -734,576 +744,586 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4">
-        <v>45681.23341435185</v>
+        <v>46019.217986111114</v>
       </c>
       <c r="B8" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
-        <v>45681.16532407407</v>
+        <v>45994.45385416667</v>
       </c>
       <c r="B9" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
-        <v>45679.995092592595</v>
+        <v>45993.10429398148</v>
       </c>
       <c r="B10" s="5">
         <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
-        <v>45962.09717592593</v>
+        <v>45833.89664351852</v>
       </c>
       <c r="B11" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4">
-        <v>45952.479050925926</v>
+        <v>45961.168032407404</v>
       </c>
       <c r="B12" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4">
-        <v>45959.712164351855</v>
+        <v>46019.199212962965</v>
       </c>
       <c r="B13" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
-        <v>45924.06623842593</v>
+        <v>45681.16532407407</v>
       </c>
       <c r="B14" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4">
-        <v>45870.10978009259</v>
+        <v>45962.09717592593</v>
       </c>
       <c r="B15" s="5">
         <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4">
-        <v>45961.53792824074</v>
+        <v>45959.712164351855</v>
       </c>
       <c r="B16" s="5">
         <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4">
-        <v>45653.15636574074</v>
+        <v>45924.06623842593</v>
       </c>
       <c r="B17" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4">
-        <v>45679.996030092596</v>
+        <v>45870.10978009259</v>
       </c>
       <c r="B18" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>26</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E18" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4">
-        <v>45865.88695601852</v>
+        <v>45992.50818287037</v>
       </c>
       <c r="B19" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4">
-        <v>45716.53192129629</v>
+        <v>46019.731990740744</v>
       </c>
       <c r="B20" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4">
-        <v>45648.90494212963</v>
+        <v>45992.51511574074</v>
       </c>
       <c r="B21" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4">
-        <v>45952.01671296296</v>
+        <v>45653.15636574074</v>
       </c>
       <c r="B22" s="5">
         <v>15</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4">
-        <v>45956.927349537036</v>
+        <v>45679.996030092596</v>
       </c>
       <c r="B23" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4">
-        <v>45649.75456018518</v>
+        <v>46019.07986111111</v>
       </c>
       <c r="B24" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4">
-        <v>45775.36515046296</v>
+        <v>45648.90494212963</v>
       </c>
       <c r="B25" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E25" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4">
-        <v>45952.006261574075</v>
+        <v>46019.113657407404</v>
       </c>
       <c r="B26" s="5">
         <v>14</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E26" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4">
-        <v>45930.54467592593</v>
+        <v>45956.927349537036</v>
       </c>
       <c r="B27" s="5">
         <v>14</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E27" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4">
-        <v>45715.48201388889</v>
+        <v>45864.11922453704</v>
       </c>
       <c r="B28" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>38</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="4">
-        <v>45798.212233796294</v>
+        <v>45775.36515046296</v>
       </c>
       <c r="B29" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="4">
-        <v>45923.70465277778</v>
+        <v>45952.006261574075</v>
       </c>
       <c r="B30" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E30" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="4">
-        <v>45960.80255787037</v>
+        <v>45930.54467592593</v>
       </c>
       <c r="B31" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E31" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="4">
-        <v>45952.697847222225</v>
+        <v>45715.48201388889</v>
       </c>
       <c r="B32" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="4">
-        <v>45960.78246527778</v>
+        <v>45798.212233796294</v>
       </c>
       <c r="B33" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="4">
-        <v>45805.79975694444</v>
+        <v>45993.95980324074</v>
       </c>
       <c r="B34" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="4">
-        <v>45959.88072916667</v>
+        <v>45648.05907407407</v>
       </c>
       <c r="B35" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="E35" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="4">
-        <v>45961.01037037037</v>
+        <v>45655.82543981481</v>
       </c>
       <c r="B36" s="5">
         <v>14</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="21">
+        <v>49</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="4">
-        <v>45952.00587962963</v>
+        <v>45992.55039351852</v>
       </c>
       <c r="B37" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="4">
-        <v>45956.38789351852</v>
+        <v>45952.44699074074</v>
       </c>
       <c r="B38" s="5">
         <v>13</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="4">
-        <v>45833.697858796295</v>
+        <v>45715.483877314815</v>
       </c>
       <c r="B39" s="5">
         <v>13</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="4">
-        <v>45932.636400462965</v>
+        <v>45992.5705787037</v>
       </c>
       <c r="B40" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="4">
-        <v>45648.05907407407</v>
+        <v>45959.88072916667</v>
       </c>
       <c r="B41" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="4">
-        <v>45655.82543981481</v>
+        <v>45961.01037037037</v>
       </c>
       <c r="B42" s="5">
         <v>14</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="4">
-        <v>45952.44699074074</v>
+        <v>45833.697858796295</v>
       </c>
       <c r="B43" s="5">
         <v>13</v>
       </c>
       <c r="C43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="E43" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="4">
-        <v>45715.483877314815</v>
+        <v>45932.636400462965</v>
       </c>
       <c r="B44" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="7"/>

</xml_diff>